<commit_message>
09/24/2020 - pushed completed project after fixed the TC_5-FDR_E2E-FDR-2938-SYSTEM ADMIN REFERENCE DATA
</commit_message>
<xml_diff>
--- a/Data Files/End_2_End/FDR_End_End_Receipt.xlsx
+++ b/Data Files/End_2_End/FDR_End_End_Receipt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fdr-automation-develop_08_25_2020\Data Files\End_2_End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FDR-Katalon-Regression\Data Files\End_2_End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D52A99A-B45C-48C8-BC70-059A2B2243B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9A190A-1124-44C8-93A6-69258C51F963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FDR_End_End_Receipt" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Manual?</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>controllerReceiptInput</t>
-  </si>
-  <si>
-    <t>09/30/2020</t>
   </si>
   <si>
     <t>DI0000018</t>
@@ -208,7 +205,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00%_);\(0.00%\)"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -344,9 +341,9 @@
     <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency 2" xfId="3" xr:uid="{01A6C98E-0568-4F3D-A49B-2B27DBDBA2C8}"/>
@@ -633,7 +630,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,12 +771,12 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>53</v>
+      <c r="A2" s="24">
+        <v>44116</v>
       </c>
       <c r="B2" s="24">
         <f>A2+2</f>
-        <v>44106</v>
+        <v>44118</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -872,15 +869,15 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>53</v>
+      <c r="A3" s="24">
+        <v>44116</v>
       </c>
       <c r="B3" s="24">
         <f>A3+2</f>
-        <v>44106</v>
+        <v>44118</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>4</v>

</xml_diff>